<commit_message>
Resolvido conflito em TE_Disparo.xlsx
</commit_message>
<xml_diff>
--- a/TE_Disparo.xlsx
+++ b/TE_Disparo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Arquivos\Desenvolvimento\EnviarEmail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AED2B2-F6F4-4EF6-B557-F3655A1E5116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BF9B1E-EBC9-4860-AE20-3899BF391402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
   <si>
     <t>Cliente</t>
   </si>
@@ -340,9 +340,6 @@
     <t>comercial_sp@ouronegro.com,comercialcorporativo2@ouronegro.com,sac9_sp@ouronegro.com,ouronegro@ouronegro.com,comercialcorporativo2@ouronegro.com,coletas_fl@ouronegro.com,sac_ct@ouronegro.com,sac_pgz@ouronegro.com</t>
   </si>
   <si>
-    <t>SC</t>
-  </si>
-  <si>
     <t>01/03/2024</t>
   </si>
   <si>
@@ -422,18 +419,6 @@
   </si>
   <si>
     <t>05/03/2024 08:43:36</t>
-  </si>
-  <si>
-    <t>TERRAPLANAGEM BANDEIRANTE LTDA</t>
-  </si>
-  <si>
-    <t>BANDEIRANTE</t>
-  </si>
-  <si>
-    <t>29/02/2024 08:32:27</t>
-  </si>
-  <si>
-    <t>Previsão de entrega: 07/03/24 - verificando status de entrega com a transportadora</t>
   </si>
   <si>
     <t>logistica@bmchyundai.com.br,osc.ocorrencias@twl.com.br,moema.dullius@twl.com.br,gabriel.zang@twtransportes.com.br,aline.silveira@twtransportes.com.br,tabela@twtransportes.com.br,cta.ocorrencias@twtransportes.com.br,bid@twtransportes.com.br,coletas@twtransportes.com.br,rayane.severo@twl.com.br</t>
@@ -899,11 +884,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -989,7 +974,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="10">
         <v>57820171049</v>
@@ -998,22 +983,22 @@
         <v>138464</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="G2" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J2" s="10">
         <v>7</v>
@@ -1031,7 +1016,7 @@
         <v>138464</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P2" s="17"/>
       <c r="S2" s="12" t="str">
@@ -1041,7 +1026,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="10">
         <v>27487509000167</v>
@@ -1050,22 +1035,22 @@
         <v>138376</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>54</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J3" s="10">
         <v>8</v>
@@ -1083,7 +1068,7 @@
         <v>138376</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P3" s="17"/>
       <c r="S3" s="12" t="str">
@@ -1093,7 +1078,7 @@
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="10">
         <v>60477199100</v>
@@ -1102,22 +1087,22 @@
         <v>138556</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J4" s="10">
         <v>7</v>
@@ -1135,7 +1120,7 @@
         <v>138556</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P4" s="9"/>
       <c r="S4" s="12" t="str">
@@ -1145,7 +1130,7 @@
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="10">
         <v>29146234000123</v>
@@ -1154,22 +1139,22 @@
         <v>138635</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J5" s="10">
         <v>3</v>
@@ -1187,64 +1172,12 @@
         <v>138635</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P5" s="17"/>
       <c r="S5" s="12" t="str">
         <f>VLOOKUP(H5,Contatos!A:B,2,0)</f>
         <v>interior.bhz@movvi.com.br,logistica@bmchyundai.com.br,michele.henriques@movvi.com.br,pendencia2interior.bhz@movvi.com.br,entrega.vix@movvi.com.br</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="10">
-        <v>32455691000104</v>
-      </c>
-      <c r="C6" s="10">
-        <v>138471</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" s="10">
-        <v>7</v>
-      </c>
-      <c r="K6" s="10">
-        <v>5</v>
-      </c>
-      <c r="L6" s="10">
-        <v>13</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="19">
-        <v>138471</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="P6" s="17"/>
-      <c r="S6" s="12" t="str">
-        <f>VLOOKUP(H6,Contatos!A:B,2,0)</f>
-        <v>logistica@bmchyundai.com.br,osc.ocorrencias@twl.com.br,moema.dullius@twl.com.br,gabriel.zang@twtransportes.com.br,aline.silveira@twtransportes.com.br,tabela@twtransportes.com.br,cta.ocorrencias@twtransportes.com.br,bid@twtransportes.com.br,coletas@twtransportes.com.br,rayane.severo@twl.com.br</v>
       </c>
     </row>
   </sheetData>
@@ -1252,7 +1185,7 @@
   <customSheetViews>
     <customSheetView guid="{F4E47935-89ED-4945-9CD3-947E4497D6BA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="B1:P984" xr:uid="{66DBC575-835F-4FA0-8B2E-FE59D52D5D2B}"/>
+      <autoFilter ref="B1:P984" xr:uid="{D78870C8-A5E1-4129-AB10-B61CBBF9E092}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="810247410"/>
@@ -1267,14 +1200,14 @@
   <conditionalFormatting sqref="C2:C3">
     <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C6">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="C4:C5">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C5">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6 C2:C3">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1331,7 +1264,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1672,10 +1605,10 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mudança na tratativa dos dados da planilha
</commit_message>
<xml_diff>
--- a/TE_Disparo.xlsx
+++ b/TE_Disparo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Arquivos\Desenvolvimento\EnviarEmail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BF9B1E-EBC9-4860-AE20-3899BF391402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67813EF2-9E28-4504-A68A-B2274175E78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Contatos" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$1</definedName>
-    <definedName name="Z_F4E47935_89ED_4945_9CD3_947E4497D6BA_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$B$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$1</definedName>
+    <definedName name="Z_F4E47935_89ED_4945_9CD3_947E4497D6BA_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$B$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
   <si>
     <t>Cliente</t>
   </si>
@@ -340,91 +340,70 @@
     <t>comercial_sp@ouronegro.com,comercialcorporativo2@ouronegro.com,sac9_sp@ouronegro.com,ouronegro@ouronegro.com,comercialcorporativo2@ouronegro.com,coletas_fl@ouronegro.com,sac_ct@ouronegro.com,sac_pgz@ouronegro.com</t>
   </si>
   <si>
-    <t>01/03/2024</t>
-  </si>
-  <si>
     <t>TW Transporte</t>
   </si>
   <si>
-    <t>05/03/2024</t>
-  </si>
-  <si>
-    <t>CESAR ANTONIO PRZYCZYNSKI</t>
-  </si>
-  <si>
-    <t>Goiânia</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
-    <t>CHEGADA EM UNIDADE [Marcar Entrega]</t>
-  </si>
-  <si>
-    <t>29/02/2024 08:32:26</t>
-  </si>
-  <si>
-    <t>Previsão de entrega: 06/03/24 - verificando status de entrega com a transportadora</t>
-  </si>
-  <si>
-    <t>PAULO MARCOS DIAS DOS SANTOS</t>
-  </si>
-  <si>
-    <t>Rolim de Moura</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>ENVIO PARA REDESPACHO [Marcar Entrega]</t>
-  </si>
-  <si>
-    <t>03/04/2024 16:49:00</t>
-  </si>
-  <si>
-    <t>28/02/2024 11:23:00</t>
-  </si>
-  <si>
-    <t>Previsao de entrega: 07/03/24 - verificando status da entrega com a transportadora</t>
-  </si>
-  <si>
-    <t>ROGERIO LUIS HOFFMANN</t>
-  </si>
-  <si>
-    <t>Chapadão do Sul</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>CHEGADA EM UNIDADE (84) [Marcar Entrega]</t>
-  </si>
-  <si>
-    <t>01/03/2024 08:39:14</t>
-  </si>
-  <si>
-    <t>DARIO PEREIRA DOS SANTOS 08190692720</t>
-  </si>
-  <si>
-    <t>Serra</t>
-  </si>
-  <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>SP3077232E [Marcar Entrega]</t>
-  </si>
-  <si>
-    <t>03/05/2024 21:20:47</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:36</t>
-  </si>
-  <si>
     <t>logistica@bmchyundai.com.br,osc.ocorrencias@twl.com.br,moema.dullius@twl.com.br,gabriel.zang@twtransportes.com.br,aline.silveira@twtransportes.com.br,tabela@twtransportes.com.br,cta.ocorrencias@twtransportes.com.br,bid@twtransportes.com.br,coletas@twtransportes.com.br,rayane.severo@twl.com.br</t>
   </si>
   <si>
     <t>interior.bhz@movvi.com.br,logistica@bmchyundai.com.br,michele.henriques@movvi.com.br,pendencia2interior.bhz@movvi.com.br,entrega.vix@movvi.com.br</t>
+  </si>
+  <si>
+    <t>Rodonaves-SANTO ANTONIO DO MONTE</t>
+  </si>
+  <si>
+    <t>AWB EM VIAGEM [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PEDRO CLEBER DOS SANTOS</t>
+  </si>
+  <si>
+    <t>01426986521</t>
+  </si>
+  <si>
+    <t>Belém</t>
+  </si>
+  <si>
+    <t>06/03/2024</t>
+  </si>
+  <si>
+    <t>06/03/2024 15:19:05</t>
+  </si>
+  <si>
+    <t>Previsao de entrega: 14/03/24 - verificando status de entrega com a transportadora</t>
+  </si>
+  <si>
+    <t>LUIZ CARLOS SAO MATEUS</t>
+  </si>
+  <si>
+    <t>01016179502</t>
+  </si>
+  <si>
+    <t>Barreiras</t>
+  </si>
+  <si>
+    <t>SAIDA DE UNIDADE [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>11/03/2024</t>
+  </si>
+  <si>
+    <t>08/03/2024 08:24:38</t>
+  </si>
+  <si>
+    <t>Previsão de entrega: 14/03/24 - verificando status de entrega com a transportadora</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -612,57 +591,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{5FA7E8DA-F6F0-4F04-83F8-2C6B95C1A608}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{DF46CC84-00C7-4CC3-95B8-8980027DCBB3}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -884,11 +813,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -897,23 +826,23 @@
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" customWidth="1"/>
-    <col min="11" max="12" width="8.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="30.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" customWidth="1"/>
+    <col min="5" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="13" width="8.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="30.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -930,262 +859,167 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="10">
-        <v>57820171049</v>
+        <v>106</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="C2" s="10">
-        <v>138464</v>
+        <v>138732</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="H2" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" s="10">
+        <v>9</v>
+      </c>
+      <c r="L2" s="10">
+        <v>5</v>
+      </c>
+      <c r="M2" s="10">
+        <v>13</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="19">
+        <v>138732</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="T2" s="12" t="str">
+        <f>VLOOKUP(I2,Contatos!A:B,2,0)</f>
+        <v>gsdr@braspress.com,sdr.vendas01@braspress.com,sdr.vendas11@braspress.com,logistica@bmchyundai.com.br,oper.iara@braspress.com,oper.marial@braspress.com,oper.diegos@braspress.com,oper.patricia@braspress.com,oper.marial@braspress.com</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="10">
+        <v>138861</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="F3" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" s="10">
+      <c r="J3" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K3" s="10">
         <v>7</v>
       </c>
-      <c r="K2" s="10">
+      <c r="L3" s="10">
         <v>5</v>
       </c>
-      <c r="L2" s="10">
+      <c r="M3" s="10">
         <v>13</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="19">
-        <v>138464</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="P2" s="17"/>
-      <c r="S2" s="12" t="str">
-        <f>VLOOKUP(H2,Contatos!A:B,2,0)</f>
+      <c r="O3" s="19">
+        <v>138861</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q3" s="17"/>
+      <c r="T3" s="12" t="str">
+        <f>VLOOKUP(I3,Contatos!A:B,2,0)</f>
         <v>parceiros@accertlogistica.com.br,sac@accertlogistica.com.br,atendimentosao@accertlogistica.com.br,accert007@accertlogistica.com.br,operacionalgyn@accertlogistica.com.br,accertgyn@accertlogistica.com.br,expedicaogyn@accertlogistica.com.br,supervisaosac@accertlogistica.com.br,logistica@bmchyundai.com.br</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="10">
-        <v>27487509000167</v>
-      </c>
-      <c r="C3" s="10">
-        <v>138376</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="10">
-        <v>8</v>
-      </c>
-      <c r="K3" s="10">
-        <v>5</v>
-      </c>
-      <c r="L3" s="10">
-        <v>13</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="19">
-        <v>138376</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="P3" s="17"/>
-      <c r="S3" s="12" t="str">
-        <f>VLOOKUP(H3,Contatos!A:B,2,0)</f>
-        <v>sac@aviatcargo.com.br,gimailton@aviatcargo.com.br,logistica@bmchyundai.com.br</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="10">
-        <v>60477199100</v>
-      </c>
-      <c r="C4" s="10">
-        <v>138556</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" s="10">
-        <v>7</v>
-      </c>
-      <c r="K4" s="10">
-        <v>6</v>
-      </c>
-      <c r="L4" s="10">
-        <v>11</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="19">
-        <v>138556</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="P4" s="9"/>
-      <c r="S4" s="12" t="str">
-        <f>VLOOKUP(H4,Contatos!A:B,2,0)</f>
-        <v>saopaulo@kmtransportes.com.br,comercial01@kmtransportes.com.br,contato@kmtransportes.com.br,thiago@kmtransportes.com.br,entrega3@kmtransportes.com.br,logistica@bmchyundai.com.br,controle03@kmtransportes.com.br</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="10">
-        <v>29146234000123</v>
-      </c>
-      <c r="C5" s="10">
-        <v>138635</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="10">
-        <v>3</v>
-      </c>
-      <c r="K5" s="10">
-        <v>2</v>
-      </c>
-      <c r="L5" s="10">
-        <v>8</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="19">
-        <v>138635</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="P5" s="17"/>
-      <c r="S5" s="12" t="str">
-        <f>VLOOKUP(H5,Contatos!A:B,2,0)</f>
-        <v>interior.bhz@movvi.com.br,logistica@bmchyundai.com.br,michele.henriques@movvi.com.br,pendencia2interior.bhz@movvi.com.br,entrega.vix@movvi.com.br</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:S1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{F4E47935-89ED-4945-9CD3-947E4497D6BA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="B1:P984" xr:uid="{D78870C8-A5E1-4129-AB10-B61CBBF9E092}"/>
+      <autoFilter ref="B1:P984" xr:uid="{57748877-19EC-4BC2-BC43-7174D9887ABA}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="810247410"/>
@@ -1194,20 +1028,7 @@
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C5">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C5">
-    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1216,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24EADED-37E2-461D-9B5D-03B866E4EAAD}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1085,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1492,123 +1313,131 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>32</v>
+      <c r="A34" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B40" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B41" s="14" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B43" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B44" s="14" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="14" t="s">
         <v>100</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1620,23 +1449,23 @@
     <hyperlink ref="B4" r:id="rId5" xr:uid="{E69C717B-97F8-405E-9858-72B74DE7203D}"/>
     <hyperlink ref="B8" r:id="rId6" display="rosimeire.sousa@atualcargas.com.br,iara.emina@atualcargas.com.br,tracking@atualcargas.com.br,logistica@bmchyundai.com.br,elenita.costa@atualcargas.com.br,leonilda.carvalho@atualcargas.com.br,ugleiton.oliveira@atualcargas.com.br,gabriela.costa@atualcargas.com.br,ilka.brito@atualcargas.com.br,martin.silva@atualcargas.com.br,jackson.silva@atualcargas.com.br,gustavo.araujo@atualcargas.com.br,raimunda.fonseca@atualcargas.com.br,estevam.santos@atualcargas.com.br,thalita.almeida@atualcargas.com.br" xr:uid="{1E040898-256F-4A17-B154-92CAD9131189}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{77F7697B-C1DD-4F75-A5A2-82094054E5D8}"/>
-    <hyperlink ref="B36" r:id="rId8" xr:uid="{F944992F-DDE3-49B1-953C-C668A54D9183}"/>
-    <hyperlink ref="B35" r:id="rId9" xr:uid="{CC0F1BBF-8852-41FD-B1C2-74CE247E3361}"/>
-    <hyperlink ref="B34" r:id="rId10" xr:uid="{FF4183ED-7929-4283-A254-257EEA4E03EF}"/>
+    <hyperlink ref="B37" r:id="rId8" xr:uid="{F944992F-DDE3-49B1-953C-C668A54D9183}"/>
+    <hyperlink ref="B36" r:id="rId9" xr:uid="{CC0F1BBF-8852-41FD-B1C2-74CE247E3361}"/>
+    <hyperlink ref="B35" r:id="rId10" xr:uid="{FF4183ED-7929-4283-A254-257EEA4E03EF}"/>
     <hyperlink ref="B10" r:id="rId11" xr:uid="{E7D613A8-0EB3-4FE2-BA7C-44BF47275FEC}"/>
     <hyperlink ref="B11:B12" r:id="rId12" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{77B88548-4559-44D1-8C35-F51DCD1C97BA}"/>
     <hyperlink ref="B11" r:id="rId13" xr:uid="{2A1C15B4-2429-44BD-8ED1-D8B47516B172}"/>
     <hyperlink ref="B12" r:id="rId14" xr:uid="{57019169-44EE-4444-AFC1-B51E5BCFD7C4}"/>
-    <hyperlink ref="B37" r:id="rId15" xr:uid="{02AC1819-F793-471B-99BE-F5C5A8264FD4}"/>
-    <hyperlink ref="B38" r:id="rId16" xr:uid="{72E3C1F1-90CE-4A24-9946-9B369C03205F}"/>
-    <hyperlink ref="B39" r:id="rId17" xr:uid="{629AAD1C-A6D4-4091-94F7-F1CA0F2CEC92}"/>
-    <hyperlink ref="B40" r:id="rId18" display="COMERCIAL1.PVH@carvalima.com.br,COLETAS.PVH@carvalima.com.br,recepcao01.pvh@carvalima.com.br,comercial1.mtz@carvalima.com.br,supervisorcomercial.sao@carvalima.com.br,qualidade.06@carvalima.com.br,logistica@bmchyundai.com.br,comercial04.sao@carvalima.com.br" xr:uid="{5D5EEBBF-D277-4B63-98A3-B9A27D5E0D9F}"/>
-    <hyperlink ref="B42" r:id="rId19" xr:uid="{E5F32D62-0B17-4B45-B2A3-2D023E729396}"/>
+    <hyperlink ref="B38" r:id="rId15" xr:uid="{02AC1819-F793-471B-99BE-F5C5A8264FD4}"/>
+    <hyperlink ref="B39" r:id="rId16" xr:uid="{72E3C1F1-90CE-4A24-9946-9B369C03205F}"/>
+    <hyperlink ref="B40" r:id="rId17" xr:uid="{629AAD1C-A6D4-4091-94F7-F1CA0F2CEC92}"/>
+    <hyperlink ref="B41" r:id="rId18" display="COMERCIAL1.PVH@carvalima.com.br,COLETAS.PVH@carvalima.com.br,recepcao01.pvh@carvalima.com.br,comercial1.mtz@carvalima.com.br,supervisorcomercial.sao@carvalima.com.br,qualidade.06@carvalima.com.br,logistica@bmchyundai.com.br,comercial04.sao@carvalima.com.br" xr:uid="{5D5EEBBF-D277-4B63-98A3-B9A27D5E0D9F}"/>
+    <hyperlink ref="B43" r:id="rId19" xr:uid="{E5F32D62-0B17-4B45-B2A3-2D023E729396}"/>
     <hyperlink ref="B5" r:id="rId20" xr:uid="{A49378D1-CF59-432F-87BC-FADDA1ADCFEF}"/>
-    <hyperlink ref="B43" r:id="rId21" xr:uid="{AC02CAEE-8DD6-4F16-ACB0-76F984FAFBE1}"/>
+    <hyperlink ref="B44" r:id="rId21" xr:uid="{AC02CAEE-8DD6-4F16-ACB0-76F984FAFBE1}"/>
     <hyperlink ref="B13" r:id="rId22" xr:uid="{3EA837F0-66E2-4156-B9BB-DA7F0668A51F}"/>
-    <hyperlink ref="B44:B46" r:id="rId23" display="comercial1.spo@eurekatransportes.com.br,comercial2.mtz@eurekatransportes.com.br,logistica@bmchyundai.com.br" xr:uid="{82E1075C-254C-4364-9697-D6645E98BEBF}"/>
-    <hyperlink ref="B44" r:id="rId24" xr:uid="{D1C45E40-35E8-4241-9FA0-F40E214E8BFE}"/>
+    <hyperlink ref="B45:B47" r:id="rId23" display="comercial1.spo@eurekatransportes.com.br,comercial2.mtz@eurekatransportes.com.br,logistica@bmchyundai.com.br" xr:uid="{82E1075C-254C-4364-9697-D6645E98BEBF}"/>
+    <hyperlink ref="B45" r:id="rId24" xr:uid="{D1C45E40-35E8-4241-9FA0-F40E214E8BFE}"/>
     <hyperlink ref="B14:B15" r:id="rId25" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br,rte212@rte.com.br" xr:uid="{3DC4F382-2CEB-4D6D-95C6-15F416BFD935}"/>
     <hyperlink ref="B14" r:id="rId26" xr:uid="{9A5DBEB1-6919-47CF-ADAF-1EFE76DE2724}"/>
     <hyperlink ref="B15" r:id="rId27" xr:uid="{9C135B23-10CB-4F32-9F32-201A31739938}"/>
@@ -1644,20 +1473,20 @@
     <hyperlink ref="B16" r:id="rId29" xr:uid="{47D90638-C17E-4616-907E-1410DC9F2600}"/>
     <hyperlink ref="B17" r:id="rId30" xr:uid="{761695E3-EBBF-4B6B-8B93-CDA509C4FCB6}"/>
     <hyperlink ref="B18" r:id="rId31" xr:uid="{DFB18575-65A9-45A6-8B50-31442D52221B}"/>
-    <hyperlink ref="B45" r:id="rId32" xr:uid="{21E0F332-D101-4525-BD62-334A5CB888C0}"/>
+    <hyperlink ref="B46" r:id="rId32" xr:uid="{21E0F332-D101-4525-BD62-334A5CB888C0}"/>
     <hyperlink ref="B19" r:id="rId33" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{B07A53B2-5EB4-4779-9053-8B653C0B1555}"/>
-    <hyperlink ref="B41" r:id="rId34" display="sac@aviatcargo.com.br,gimailton@aviatcargo.com.br,luiz@aviatcargo.com.br,jeferson@aviatcargo.com.br,logistica@bmchyundai.com.br" xr:uid="{E90A00DE-4BEA-452C-A492-075708FF2C27}"/>
+    <hyperlink ref="B42" r:id="rId34" display="sac@aviatcargo.com.br,gimailton@aviatcargo.com.br,luiz@aviatcargo.com.br,jeferson@aviatcargo.com.br,logistica@bmchyundai.com.br" xr:uid="{E90A00DE-4BEA-452C-A492-075708FF2C27}"/>
     <hyperlink ref="B20:B23" r:id="rId35" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{917A7F17-0DD0-4B0D-858E-0DCE0F1B6265}"/>
     <hyperlink ref="B24" r:id="rId36" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{34C67720-C5FE-4B8A-8D1F-84F5056FAC11}"/>
     <hyperlink ref="B25" r:id="rId37" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{D172D423-37C4-4355-9EAF-B678E41EA6AE}"/>
-    <hyperlink ref="B46" r:id="rId38" xr:uid="{72E020A5-0D1D-4531-8378-0755CB92368C}"/>
+    <hyperlink ref="B47" r:id="rId38" xr:uid="{72E020A5-0D1D-4531-8378-0755CB92368C}"/>
     <hyperlink ref="B26" r:id="rId39" xr:uid="{75D03518-905E-4668-A812-1B3EBEB16519}"/>
-    <hyperlink ref="B47" r:id="rId40" xr:uid="{92BA3A59-65C5-4C02-85D0-3273EB6A2DE9}"/>
+    <hyperlink ref="B48" r:id="rId40" xr:uid="{92BA3A59-65C5-4C02-85D0-3273EB6A2DE9}"/>
     <hyperlink ref="B27" r:id="rId41" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{657FCA66-C0B8-4F90-954A-B17292A42EB1}"/>
     <hyperlink ref="B28" r:id="rId42" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{F8FABE3D-DDD4-498E-AFD4-670D65AD365E}"/>
     <hyperlink ref="B29" r:id="rId43" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{1DA0F648-43F4-4BAC-B964-2E4E8E45A46C}"/>
     <hyperlink ref="B30:B31" r:id="rId44" display="juliana.laia@rte.com.br,logistica@bmchyundai.com.br," xr:uid="{D7D624D1-D205-4D61-83F2-385CCFCCE02F}"/>
-    <hyperlink ref="B48" r:id="rId45" display="logistica@bmchyundai.com.br,osc.ocorrencias@twl.com.br,moema.dullius@twl.com.br,gabriel.zang@twtransportes.com.br,aline.silveira@twtransportes.com.br,tabela@twtransportes.com.br,cta.ocorrencias@twtransportes.com.br,bid@twtransportes.com.br,coletas@twtransportes.com.br,rayane.severo@twl.com.br" xr:uid="{2F654970-9900-4279-A791-C39909CD9215}"/>
+    <hyperlink ref="B49" r:id="rId45" display="logistica@bmchyundai.com.br,osc.ocorrencias@twl.com.br,moema.dullius@twl.com.br,gabriel.zang@twtransportes.com.br,aline.silveira@twtransportes.com.br,tabela@twtransportes.com.br,cta.ocorrencias@twtransportes.com.br,bid@twtransportes.com.br,coletas@twtransportes.com.br,rayane.severo@twl.com.br" xr:uid="{2F654970-9900-4279-A791-C39909CD9215}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>